<commit_message>
Fixes typo in species name: Cottus_bairdi
</commit_message>
<xml_diff>
--- a/Data/ToolData/AquaticSpeciesList.xlsx
+++ b/Data/ToolData/AquaticSpeciesList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\GeoWET\Data\ToolData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\GeoWET\Data\ToolData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -355,9 +355,6 @@
     <t>Rhinichthys_cataractae</t>
   </si>
   <si>
-    <t>Cottus_bairdii</t>
-  </si>
-  <si>
     <t>Ichthyomyzon_greeleyi</t>
   </si>
   <si>
@@ -374,12 +371,15 @@
   </si>
   <si>
     <t>Luxilus_coccogenis</t>
+  </si>
+  <si>
+    <t>Cottus_bairdi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1325,7 +1325,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,7 +1518,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1529,7 +1529,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1554,7 +1554,7 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1593,7 +1593,7 @@
         <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1640,7 +1640,7 @@
         <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1676,7 +1676,7 @@
         <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1704,7 +1704,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E30">
         <v>1</v>

</xml_diff>